<commit_message>
Date conversions in the output
</commit_message>
<xml_diff>
--- a/Misc/2019_to_10_2020_2.xlsx
+++ b/Misc/2019_to_10_2020_2.xlsx
@@ -3613,13 +3613,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3642,8 +3647,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4036,7 +4042,7 @@
       <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L2" t="s">
@@ -4100,7 +4106,7 @@
       <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L3"/>
@@ -4158,7 +4164,7 @@
       <c r="J4" t="s">
         <v>42</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L4"/>
@@ -4216,7 +4222,7 @@
       <c r="J5" t="s">
         <v>53</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5" s="1" t="n">
         <v>43887</v>
       </c>
       <c r="L5"/>
@@ -4274,7 +4280,7 @@
       <c r="J6" t="s">
         <v>64</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="1" t="n">
         <v>43889</v>
       </c>
       <c r="L6"/>
@@ -4332,7 +4338,7 @@
       <c r="J7" t="s">
         <v>76</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7" s="1" t="n">
         <v>43889</v>
       </c>
       <c r="L7"/>
@@ -4390,7 +4396,7 @@
       <c r="J8" t="s">
         <v>87</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L8"/>
@@ -4448,7 +4454,7 @@
       <c r="J9" t="s">
         <v>98</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9" s="1" t="n">
         <v>43895</v>
       </c>
       <c r="L9"/>
@@ -4504,7 +4510,7 @@
       <c r="J10" t="s">
         <v>108</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10" s="1" t="n">
         <v>43901</v>
       </c>
       <c r="L10"/>
@@ -4564,7 +4570,7 @@
       <c r="J11" t="s">
         <v>119</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K11" s="1" t="n">
         <v>43942</v>
       </c>
       <c r="L11"/>
@@ -4622,7 +4628,7 @@
       <c r="J12" t="s">
         <v>130</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K12" s="1" t="n">
         <v>43948</v>
       </c>
       <c r="L12" t="s">
@@ -4682,7 +4688,7 @@
       <c r="J13" t="s">
         <v>141</v>
       </c>
-      <c r="K13" t="n">
+      <c r="K13" s="1" t="n">
         <v>43949</v>
       </c>
       <c r="L13"/>
@@ -4740,7 +4746,7 @@
       <c r="J14" t="s">
         <v>130</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K14" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="L14"/>
@@ -4800,7 +4806,7 @@
       <c r="J15" t="s">
         <v>76</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K15" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="L15"/>
@@ -4862,7 +4868,7 @@
       <c r="J16" t="s">
         <v>76</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K16" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="L16"/>
@@ -4924,7 +4930,7 @@
       <c r="J17" t="s">
         <v>76</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K17" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="L17"/>
@@ -4986,7 +4992,7 @@
       <c r="J18" t="s">
         <v>76</v>
       </c>
-      <c r="K18" t="n">
+      <c r="K18" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="L18"/>
@@ -5048,7 +5054,7 @@
       <c r="J19" t="s">
         <v>177</v>
       </c>
-      <c r="K19" t="n">
+      <c r="K19" s="1" t="n">
         <v>43997</v>
       </c>
       <c r="L19"/>
@@ -5110,7 +5116,7 @@
       <c r="J20" t="s">
         <v>184</v>
       </c>
-      <c r="K20" t="n">
+      <c r="K20" s="1" t="n">
         <v>43997</v>
       </c>
       <c r="L20"/>
@@ -5172,7 +5178,7 @@
       <c r="J21" t="s">
         <v>186</v>
       </c>
-      <c r="K21" t="n">
+      <c r="K21" s="1" t="n">
         <v>43997</v>
       </c>
       <c r="L21"/>
@@ -5234,7 +5240,7 @@
       <c r="J22" t="s">
         <v>192</v>
       </c>
-      <c r="K22" t="n">
+      <c r="K22" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L22"/>
@@ -5296,7 +5302,7 @@
       <c r="J23" t="s">
         <v>199</v>
       </c>
-      <c r="K23" t="n">
+      <c r="K23" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L23"/>
@@ -5358,7 +5364,7 @@
       <c r="J24" t="s">
         <v>199</v>
       </c>
-      <c r="K24" t="n">
+      <c r="K24" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L24"/>
@@ -5420,7 +5426,7 @@
       <c r="J25" t="s">
         <v>199</v>
       </c>
-      <c r="K25" t="n">
+      <c r="K25" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L25"/>
@@ -5482,7 +5488,7 @@
       <c r="J26" t="s">
         <v>201</v>
       </c>
-      <c r="K26" t="n">
+      <c r="K26" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L26"/>
@@ -5544,7 +5550,7 @@
       <c r="J27" t="s">
         <v>201</v>
       </c>
-      <c r="K27" t="n">
+      <c r="K27" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L27"/>
@@ -5606,7 +5612,7 @@
       <c r="J28" t="s">
         <v>203</v>
       </c>
-      <c r="K28" t="n">
+      <c r="K28" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L28"/>
@@ -5668,7 +5674,7 @@
       <c r="J29" t="s">
         <v>205</v>
       </c>
-      <c r="K29" t="n">
+      <c r="K29" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L29"/>
@@ -5726,7 +5732,7 @@
       <c r="J30" t="s">
         <v>211</v>
       </c>
-      <c r="K30" t="n">
+      <c r="K30" s="1" t="n">
         <v>44020</v>
       </c>
       <c r="L30"/>
@@ -5784,7 +5790,7 @@
       <c r="J31" t="s">
         <v>218</v>
       </c>
-      <c r="K31" t="n">
+      <c r="K31" s="1" t="n">
         <v>44020</v>
       </c>
       <c r="L31"/>
@@ -5844,7 +5850,7 @@
       <c r="J32" t="s">
         <v>225</v>
       </c>
-      <c r="K32" t="n">
+      <c r="K32" s="1" t="n">
         <v>44027</v>
       </c>
       <c r="L32"/>
@@ -5904,7 +5910,7 @@
       <c r="J33" t="s">
         <v>199</v>
       </c>
-      <c r="K33" t="n">
+      <c r="K33" s="1" t="n">
         <v>44077</v>
       </c>
       <c r="L33"/>
@@ -5964,7 +5970,7 @@
       <c r="J34" t="s">
         <v>199</v>
       </c>
-      <c r="K34" t="n">
+      <c r="K34" s="1" t="n">
         <v>44077</v>
       </c>
       <c r="L34"/>
@@ -6028,7 +6034,7 @@
       <c r="J35" t="s">
         <v>22</v>
       </c>
-      <c r="K35" t="n">
+      <c r="K35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L35" t="s">
@@ -6090,7 +6096,7 @@
       <c r="J36" t="s">
         <v>244</v>
       </c>
-      <c r="K36" t="n">
+      <c r="K36" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L36"/>
@@ -6150,7 +6156,7 @@
       <c r="J37" t="s">
         <v>256</v>
       </c>
-      <c r="K37" t="n">
+      <c r="K37" s="1" t="n">
         <v>43882</v>
       </c>
       <c r="L37"/>
@@ -6210,7 +6216,7 @@
       <c r="J38" t="s">
         <v>262</v>
       </c>
-      <c r="K38" t="n">
+      <c r="K38" s="1" t="n">
         <v>43882</v>
       </c>
       <c r="L38"/>
@@ -6268,7 +6274,7 @@
       <c r="J39" t="s">
         <v>268</v>
       </c>
-      <c r="K39" t="n">
+      <c r="K39" s="1" t="n">
         <v>43885</v>
       </c>
       <c r="L39"/>
@@ -6324,7 +6330,7 @@
       <c r="J40" t="s">
         <v>278</v>
       </c>
-      <c r="K40" t="n">
+      <c r="K40" s="1" t="n">
         <v>43888</v>
       </c>
       <c r="L40"/>
@@ -6382,7 +6388,7 @@
       <c r="J41" t="s">
         <v>289</v>
       </c>
-      <c r="K41" t="n">
+      <c r="K41" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L41"/>
@@ -6438,7 +6444,7 @@
       <c r="J42" t="s">
         <v>295</v>
       </c>
-      <c r="K42" t="n">
+      <c r="K42" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L42"/>
@@ -6494,7 +6500,7 @@
       <c r="J43" t="s">
         <v>297</v>
       </c>
-      <c r="K43" t="n">
+      <c r="K43" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L43"/>
@@ -6550,7 +6556,7 @@
       <c r="J44" t="s">
         <v>299</v>
       </c>
-      <c r="K44" t="n">
+      <c r="K44" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L44"/>
@@ -6606,7 +6612,7 @@
       <c r="J45" t="s">
         <v>305</v>
       </c>
-      <c r="K45" t="n">
+      <c r="K45" s="1" t="n">
         <v>43894</v>
       </c>
       <c r="L45"/>
@@ -6660,7 +6666,7 @@
       <c r="J46" t="s">
         <v>130</v>
       </c>
-      <c r="K46" t="n">
+      <c r="K46" s="1" t="n">
         <v>43896</v>
       </c>
       <c r="L46"/>
@@ -6716,7 +6722,7 @@
       <c r="J47" t="s">
         <v>318</v>
       </c>
-      <c r="K47" t="n">
+      <c r="K47" s="1" t="n">
         <v>43896</v>
       </c>
       <c r="L47"/>
@@ -6772,7 +6778,7 @@
       <c r="J48" t="s">
         <v>322</v>
       </c>
-      <c r="K48" t="n">
+      <c r="K48" s="1" t="n">
         <v>43901</v>
       </c>
       <c r="L48"/>
@@ -6828,7 +6834,7 @@
       <c r="J49" t="s">
         <v>328</v>
       </c>
-      <c r="K49" t="n">
+      <c r="K49" s="1" t="n">
         <v>43901</v>
       </c>
       <c r="L49"/>
@@ -6884,7 +6890,7 @@
       <c r="J50" t="s">
         <v>330</v>
       </c>
-      <c r="K50" t="n">
+      <c r="K50" s="1" t="n">
         <v>43901</v>
       </c>
       <c r="L50"/>
@@ -6942,7 +6948,7 @@
       <c r="J51" t="s">
         <v>262</v>
       </c>
-      <c r="K51" t="n">
+      <c r="K51" s="1" t="n">
         <v>43903</v>
       </c>
       <c r="L51"/>
@@ -7000,7 +7006,7 @@
       <c r="J52" t="s">
         <v>199</v>
       </c>
-      <c r="K52" t="n">
+      <c r="K52" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="L52"/>
@@ -7060,7 +7066,7 @@
       <c r="J53" t="s">
         <v>356</v>
       </c>
-      <c r="K53" t="n">
+      <c r="K53" s="1" t="n">
         <v>43913</v>
       </c>
       <c r="L53"/>
@@ -7120,7 +7126,7 @@
       <c r="J54" t="s">
         <v>369</v>
       </c>
-      <c r="K54" t="n">
+      <c r="K54" s="1" t="n">
         <v>43922</v>
       </c>
       <c r="L54"/>
@@ -7178,7 +7184,7 @@
       <c r="J55" t="s">
         <v>379</v>
       </c>
-      <c r="K55" t="n">
+      <c r="K55" s="1" t="n">
         <v>43929</v>
       </c>
       <c r="L55"/>
@@ -7234,7 +7240,7 @@
       <c r="J56" t="s">
         <v>389</v>
       </c>
-      <c r="K56" t="n">
+      <c r="K56" s="1" t="n">
         <v>44007</v>
       </c>
       <c r="L56"/>
@@ -7294,7 +7300,7 @@
       <c r="J57" t="s">
         <v>399</v>
       </c>
-      <c r="K57" t="n">
+      <c r="K57" s="1" t="n">
         <v>44013</v>
       </c>
       <c r="L57"/>
@@ -7352,7 +7358,7 @@
       <c r="J58" t="s">
         <v>408</v>
       </c>
-      <c r="K58" t="n">
+      <c r="K58" s="1" t="n">
         <v>44104</v>
       </c>
       <c r="L58"/>
@@ -7410,7 +7416,7 @@
       <c r="J59" t="s">
         <v>415</v>
       </c>
-      <c r="K59" t="n">
+      <c r="K59" s="1" t="n">
         <v>44104</v>
       </c>
       <c r="L59"/>
@@ -7474,7 +7480,7 @@
       <c r="J60" t="s">
         <v>22</v>
       </c>
-      <c r="K60" t="n">
+      <c r="K60" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L60" t="s">
@@ -7536,7 +7542,7 @@
       <c r="J61" t="s">
         <v>419</v>
       </c>
-      <c r="K61" t="n">
+      <c r="K61" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L61"/>
@@ -7594,7 +7600,7 @@
       <c r="J62" t="s">
         <v>419</v>
       </c>
-      <c r="K62" t="n">
+      <c r="K62" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L62"/>
@@ -7652,7 +7658,7 @@
       <c r="J63" t="s">
         <v>419</v>
       </c>
-      <c r="K63" t="n">
+      <c r="K63" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L63"/>
@@ -7710,7 +7716,7 @@
       <c r="J64" t="s">
         <v>419</v>
       </c>
-      <c r="K64" t="n">
+      <c r="K64" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L64"/>
@@ -7768,7 +7774,7 @@
       <c r="J65" t="s">
         <v>427</v>
       </c>
-      <c r="K65" t="n">
+      <c r="K65" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L65"/>
@@ -7826,7 +7832,7 @@
       <c r="J66" t="s">
         <v>427</v>
       </c>
-      <c r="K66" t="n">
+      <c r="K66" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L66"/>
@@ -7884,7 +7890,7 @@
       <c r="J67" t="s">
         <v>427</v>
       </c>
-      <c r="K67" t="n">
+      <c r="K67" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L67"/>
@@ -7942,7 +7948,7 @@
       <c r="J68" t="s">
         <v>427</v>
       </c>
-      <c r="K68" t="n">
+      <c r="K68" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L68"/>
@@ -8000,7 +8006,7 @@
       <c r="J69" t="s">
         <v>427</v>
       </c>
-      <c r="K69" t="n">
+      <c r="K69" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L69"/>
@@ -8064,7 +8070,7 @@
       <c r="J70" t="s">
         <v>22</v>
       </c>
-      <c r="K70" t="n">
+      <c r="K70" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L70" t="s">
@@ -8126,7 +8132,7 @@
       <c r="J71" t="s">
         <v>433</v>
       </c>
-      <c r="K71" t="n">
+      <c r="K71" s="1" t="n">
         <v>43878</v>
       </c>
       <c r="L71" t="s">
@@ -8192,7 +8198,7 @@
       <c r="J72" t="s">
         <v>22</v>
       </c>
-      <c r="K72" t="n">
+      <c r="K72" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L72" t="s">
@@ -8260,7 +8266,7 @@
       <c r="J73" t="s">
         <v>22</v>
       </c>
-      <c r="K73" t="n">
+      <c r="K73" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L73" t="s">
@@ -8322,7 +8328,7 @@
       <c r="J74" t="s">
         <v>199</v>
       </c>
-      <c r="K74" t="n">
+      <c r="K74" s="1" t="n">
         <v>43882</v>
       </c>
       <c r="L74"/>
@@ -8380,7 +8386,7 @@
       <c r="J75" t="s">
         <v>451</v>
       </c>
-      <c r="K75" t="n">
+      <c r="K75" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L75"/>
@@ -8438,7 +8444,7 @@
       <c r="J76" t="s">
         <v>458</v>
       </c>
-      <c r="K76" t="n">
+      <c r="K76" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L76"/>
@@ -8496,7 +8502,7 @@
       <c r="J77" t="s">
         <v>462</v>
       </c>
-      <c r="K77" t="n">
+      <c r="K77" s="1" t="n">
         <v>43901</v>
       </c>
       <c r="L77"/>
@@ -8544,7 +8550,7 @@
       <c r="J78" t="s">
         <v>76</v>
       </c>
-      <c r="K78" t="n">
+      <c r="K78" s="1" t="n">
         <v>43901</v>
       </c>
       <c r="L78"/>
@@ -8592,7 +8598,7 @@
       <c r="J79" t="s">
         <v>466</v>
       </c>
-      <c r="K79" t="n">
+      <c r="K79" s="1" t="n">
         <v>43903</v>
       </c>
       <c r="L79"/>
@@ -8644,7 +8650,7 @@
       <c r="J80" t="s">
         <v>472</v>
       </c>
-      <c r="K80" t="n">
+      <c r="K80" s="1" t="n">
         <v>43906</v>
       </c>
       <c r="L80"/>
@@ -8704,7 +8710,7 @@
       <c r="J81" t="s">
         <v>199</v>
       </c>
-      <c r="K81" t="n">
+      <c r="K81" s="1" t="n">
         <v>43907</v>
       </c>
       <c r="L81"/>
@@ -8764,7 +8770,7 @@
       <c r="J82" t="s">
         <v>489</v>
       </c>
-      <c r="K82" t="n">
+      <c r="K82" s="1" t="n">
         <v>43907</v>
       </c>
       <c r="L82"/>
@@ -8822,7 +8828,7 @@
       <c r="J83" t="s">
         <v>493</v>
       </c>
-      <c r="K83" t="n">
+      <c r="K83" s="1" t="n">
         <v>43909</v>
       </c>
       <c r="L83"/>
@@ -8880,7 +8886,7 @@
       <c r="J84" t="s">
         <v>489</v>
       </c>
-      <c r="K84" t="n">
+      <c r="K84" s="1" t="n">
         <v>43915</v>
       </c>
       <c r="L84"/>
@@ -8938,7 +8944,7 @@
       <c r="J85" t="s">
         <v>278</v>
       </c>
-      <c r="K85" t="n">
+      <c r="K85" s="1" t="n">
         <v>43917</v>
       </c>
       <c r="L85"/>
@@ -8996,7 +9002,7 @@
       <c r="J86" t="s">
         <v>515</v>
       </c>
-      <c r="K86" t="n">
+      <c r="K86" s="1" t="n">
         <v>43917</v>
       </c>
       <c r="L86"/>
@@ -9054,7 +9060,7 @@
       <c r="J87" t="s">
         <v>199</v>
       </c>
-      <c r="K87" t="n">
+      <c r="K87" s="1" t="n">
         <v>43924</v>
       </c>
       <c r="L87"/>
@@ -9112,7 +9118,7 @@
       <c r="J88" t="s">
         <v>489</v>
       </c>
-      <c r="K88" t="n">
+      <c r="K88" s="1" t="n">
         <v>43924</v>
       </c>
       <c r="L88"/>
@@ -9172,7 +9178,7 @@
       <c r="J89" t="s">
         <v>524</v>
       </c>
-      <c r="K89" t="n">
+      <c r="K89" s="1" t="n">
         <v>43941</v>
       </c>
       <c r="L89"/>
@@ -9232,7 +9238,7 @@
       <c r="J90" t="s">
         <v>278</v>
       </c>
-      <c r="K90" t="n">
+      <c r="K90" s="1" t="n">
         <v>43941</v>
       </c>
       <c r="L90"/>
@@ -9292,7 +9298,7 @@
       <c r="J91" t="s">
         <v>532</v>
       </c>
-      <c r="K91" t="n">
+      <c r="K91" s="1" t="n">
         <v>43941</v>
       </c>
       <c r="L91"/>
@@ -9352,7 +9358,7 @@
       <c r="J92" t="s">
         <v>130</v>
       </c>
-      <c r="K92" t="n">
+      <c r="K92" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="L92"/>
@@ -9410,7 +9416,7 @@
       <c r="J93" t="s">
         <v>546</v>
       </c>
-      <c r="K93" t="n">
+      <c r="K93" s="1" t="n">
         <v>43955</v>
       </c>
       <c r="L93"/>
@@ -9468,7 +9474,7 @@
       <c r="J94" t="s">
         <v>557</v>
       </c>
-      <c r="K94" t="n">
+      <c r="K94" s="1" t="n">
         <v>43962</v>
       </c>
       <c r="L94"/>
@@ -9526,7 +9532,7 @@
       <c r="J95" t="s">
         <v>564</v>
       </c>
-      <c r="K95" t="n">
+      <c r="K95" s="1" t="n">
         <v>43962</v>
       </c>
       <c r="L95"/>
@@ -9588,7 +9594,7 @@
       <c r="J96" t="s">
         <v>76</v>
       </c>
-      <c r="K96" t="n">
+      <c r="K96" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="L96"/>
@@ -9650,7 +9656,7 @@
       <c r="J97" t="s">
         <v>76</v>
       </c>
-      <c r="K97" t="n">
+      <c r="K97" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="L97"/>
@@ -9712,7 +9718,7 @@
       <c r="J98" t="s">
         <v>76</v>
       </c>
-      <c r="K98" t="n">
+      <c r="K98" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="L98"/>
@@ -9774,7 +9780,7 @@
       <c r="J99" t="s">
         <v>76</v>
       </c>
-      <c r="K99" t="n">
+      <c r="K99" s="1" t="n">
         <v>43966</v>
       </c>
       <c r="L99"/>
@@ -9834,7 +9840,7 @@
       <c r="J100" t="s">
         <v>278</v>
       </c>
-      <c r="K100" t="n">
+      <c r="K100" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="L100"/>
@@ -9894,7 +9900,7 @@
       <c r="J101" t="s">
         <v>574</v>
       </c>
-      <c r="K101" t="n">
+      <c r="K101" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="L101"/>
@@ -9954,7 +9960,7 @@
       <c r="J102" t="s">
         <v>564</v>
       </c>
-      <c r="K102" t="n">
+      <c r="K102" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="L102"/>
@@ -10014,7 +10020,7 @@
       <c r="J103" t="s">
         <v>579</v>
       </c>
-      <c r="K103" t="n">
+      <c r="K103" s="1" t="n">
         <v>44011</v>
       </c>
       <c r="L103"/>
@@ -10072,7 +10078,7 @@
       <c r="J104" t="s">
         <v>590</v>
       </c>
-      <c r="K104" t="n">
+      <c r="K104" s="1" t="n">
         <v>44019</v>
       </c>
       <c r="L104"/>
@@ -10130,7 +10136,7 @@
       <c r="J105" t="s">
         <v>211</v>
       </c>
-      <c r="K105" t="n">
+      <c r="K105" s="1" t="n">
         <v>44020</v>
       </c>
       <c r="L105"/>
@@ -10188,7 +10194,7 @@
       <c r="J106" t="s">
         <v>218</v>
       </c>
-      <c r="K106" t="n">
+      <c r="K106" s="1" t="n">
         <v>44020</v>
       </c>
       <c r="L106"/>
@@ -10250,7 +10256,7 @@
       <c r="J107" t="s">
         <v>205</v>
       </c>
-      <c r="K107" t="n">
+      <c r="K107" s="1" t="n">
         <v>44021</v>
       </c>
       <c r="L107"/>
@@ -10312,7 +10318,7 @@
       <c r="J108" t="s">
         <v>608</v>
       </c>
-      <c r="K108" t="n">
+      <c r="K108" s="1" t="n">
         <v>44021</v>
       </c>
       <c r="L108"/>
@@ -10370,7 +10376,7 @@
       <c r="J109" t="s">
         <v>612</v>
       </c>
-      <c r="K109" t="n">
+      <c r="K109" s="1" t="n">
         <v>44021</v>
       </c>
       <c r="L109"/>
@@ -10430,7 +10436,7 @@
       <c r="J110" t="s">
         <v>295</v>
       </c>
-      <c r="K110" t="n">
+      <c r="K110" s="1" t="n">
         <v>44026</v>
       </c>
       <c r="L110"/>
@@ -10490,7 +10496,7 @@
       <c r="J111" t="s">
         <v>629</v>
       </c>
-      <c r="K111" t="n">
+      <c r="K111" s="1" t="n">
         <v>44026</v>
       </c>
       <c r="L111"/>
@@ -10548,7 +10554,7 @@
       <c r="J112" t="s">
         <v>633</v>
       </c>
-      <c r="K112" t="n">
+      <c r="K112" s="1" t="n">
         <v>44028</v>
       </c>
       <c r="L112"/>
@@ -10608,7 +10614,7 @@
       <c r="J113" t="s">
         <v>262</v>
       </c>
-      <c r="K113" t="n">
+      <c r="K113" s="1" t="n">
         <v>44032</v>
       </c>
       <c r="L113"/>
@@ -10666,7 +10672,7 @@
       <c r="J114" t="s">
         <v>652</v>
       </c>
-      <c r="K114" t="n">
+      <c r="K114" s="1" t="n">
         <v>44032</v>
       </c>
       <c r="L114"/>
@@ -10724,7 +10730,7 @@
       <c r="J115" t="s">
         <v>663</v>
       </c>
-      <c r="K115" t="n">
+      <c r="K115" s="1" t="n">
         <v>44033</v>
       </c>
       <c r="L115"/>
@@ -10782,7 +10788,7 @@
       <c r="J116" t="s">
         <v>672</v>
       </c>
-      <c r="K116" t="n">
+      <c r="K116" s="1" t="n">
         <v>44033</v>
       </c>
       <c r="L116"/>
@@ -10840,7 +10846,7 @@
       <c r="J117" t="s">
         <v>681</v>
       </c>
-      <c r="K117" t="n">
+      <c r="K117" s="1" t="n">
         <v>44034</v>
       </c>
       <c r="L117"/>
@@ -10900,7 +10906,7 @@
       <c r="J118" t="s">
         <v>689</v>
       </c>
-      <c r="K118" t="n">
+      <c r="K118" s="1" t="n">
         <v>44034</v>
       </c>
       <c r="L118"/>
@@ -10960,7 +10966,7 @@
       <c r="J119" t="s">
         <v>698</v>
       </c>
-      <c r="K119" t="n">
+      <c r="K119" s="1" t="n">
         <v>44034</v>
       </c>
       <c r="L119"/>
@@ -11018,7 +11024,7 @@
       <c r="J120" t="s">
         <v>698</v>
       </c>
-      <c r="K120" t="n">
+      <c r="K120" s="1" t="n">
         <v>44034</v>
       </c>
       <c r="L120"/>
@@ -11076,7 +11082,7 @@
       <c r="J121" t="s">
         <v>199</v>
       </c>
-      <c r="K121" t="n">
+      <c r="K121" s="1" t="n">
         <v>44046</v>
       </c>
       <c r="L121"/>
@@ -11134,7 +11140,7 @@
       <c r="J122" t="s">
         <v>262</v>
       </c>
-      <c r="K122" t="n">
+      <c r="K122" s="1" t="n">
         <v>44049</v>
       </c>
       <c r="L122"/>
@@ -11194,7 +11200,7 @@
       <c r="J123" t="s">
         <v>130</v>
       </c>
-      <c r="K123" t="n">
+      <c r="K123" s="1" t="n">
         <v>44049</v>
       </c>
       <c r="L123"/>
@@ -11252,7 +11258,7 @@
       <c r="J124" t="s">
         <v>629</v>
       </c>
-      <c r="K124" t="n">
+      <c r="K124" s="1" t="n">
         <v>44061</v>
       </c>
       <c r="L124"/>
@@ -11310,7 +11316,7 @@
       <c r="J125" t="s">
         <v>739</v>
       </c>
-      <c r="K125" t="n">
+      <c r="K125" s="1" t="n">
         <v>44062</v>
       </c>
       <c r="L125"/>
@@ -11368,7 +11374,7 @@
       <c r="J126" t="s">
         <v>130</v>
       </c>
-      <c r="K126" t="n">
+      <c r="K126" s="1" t="n">
         <v>44062</v>
       </c>
       <c r="L126"/>
@@ -11426,7 +11432,7 @@
       <c r="J127" t="s">
         <v>419</v>
       </c>
-      <c r="K127" t="n">
+      <c r="K127" s="1" t="n">
         <v>44068</v>
       </c>
       <c r="L127"/>
@@ -11484,7 +11490,7 @@
       <c r="J128" t="s">
         <v>756</v>
       </c>
-      <c r="K128" t="n">
+      <c r="K128" s="1" t="n">
         <v>44068</v>
       </c>
       <c r="L128"/>
@@ -11542,7 +11548,7 @@
       <c r="J129" t="s">
         <v>763</v>
       </c>
-      <c r="K129" t="n">
+      <c r="K129" s="1" t="n">
         <v>44068</v>
       </c>
       <c r="L129"/>
@@ -11600,7 +11606,7 @@
       <c r="J130" t="s">
         <v>767</v>
       </c>
-      <c r="K130" t="n">
+      <c r="K130" s="1" t="n">
         <v>44076</v>
       </c>
       <c r="L130"/>
@@ -11658,7 +11664,7 @@
       <c r="J131" t="s">
         <v>772</v>
       </c>
-      <c r="K131" t="n">
+      <c r="K131" s="1" t="n">
         <v>44076</v>
       </c>
       <c r="L131"/>
@@ -11716,7 +11722,7 @@
       <c r="J132" t="s">
         <v>415</v>
       </c>
-      <c r="K132" t="n">
+      <c r="K132" s="1" t="n">
         <v>44076</v>
       </c>
       <c r="L132"/>
@@ -11780,7 +11786,7 @@
       <c r="J133" t="s">
         <v>22</v>
       </c>
-      <c r="K133" t="n">
+      <c r="K133" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L133" t="s">
@@ -11844,7 +11850,7 @@
       <c r="J134" t="s">
         <v>779</v>
       </c>
-      <c r="K134" t="n">
+      <c r="K134" s="1" t="n">
         <v>43879</v>
       </c>
       <c r="L134"/>
@@ -11904,7 +11910,7 @@
       <c r="J135" t="s">
         <v>786</v>
       </c>
-      <c r="K135" t="n">
+      <c r="K135" s="1" t="n">
         <v>43879</v>
       </c>
       <c r="L135"/>
@@ -11968,7 +11974,7 @@
       <c r="J136" t="s">
         <v>22</v>
       </c>
-      <c r="K136" t="n">
+      <c r="K136" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L136" t="s">
@@ -12030,7 +12036,7 @@
       <c r="J137" t="s">
         <v>792</v>
       </c>
-      <c r="K137" t="n">
+      <c r="K137" s="1" t="n">
         <v>43879</v>
       </c>
       <c r="L137" t="s">
@@ -12096,7 +12102,7 @@
       <c r="J138" t="s">
         <v>22</v>
       </c>
-      <c r="K138" t="n">
+      <c r="K138" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L138" t="s">
@@ -12164,7 +12170,7 @@
       <c r="J139" t="s">
         <v>22</v>
       </c>
-      <c r="K139" t="n">
+      <c r="K139" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L139" t="s">
@@ -12226,7 +12232,7 @@
       <c r="J140" t="s">
         <v>801</v>
       </c>
-      <c r="K140" t="n">
+      <c r="K140" s="1" t="n">
         <v>43880</v>
       </c>
       <c r="L140"/>
@@ -12282,7 +12288,7 @@
       <c r="J141" t="s">
         <v>807</v>
       </c>
-      <c r="K141" t="n">
+      <c r="K141" s="1" t="n">
         <v>43880</v>
       </c>
       <c r="L141"/>
@@ -12344,7 +12350,7 @@
       <c r="J142" t="s">
         <v>22</v>
       </c>
-      <c r="K142" t="n">
+      <c r="K142" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L142" t="s">
@@ -12406,7 +12412,7 @@
       <c r="J143" t="s">
         <v>812</v>
       </c>
-      <c r="K143" t="n">
+      <c r="K143" s="1" t="n">
         <v>43887</v>
       </c>
       <c r="L143"/>
@@ -12462,7 +12468,7 @@
       <c r="J144" t="s">
         <v>192</v>
       </c>
-      <c r="K144" t="n">
+      <c r="K144" s="1" t="n">
         <v>43896</v>
       </c>
       <c r="L144"/>
@@ -12520,7 +12526,7 @@
       <c r="J145" t="s">
         <v>829</v>
       </c>
-      <c r="K145" t="n">
+      <c r="K145" s="1" t="n">
         <v>43902</v>
       </c>
       <c r="L145" t="s">
@@ -12580,7 +12586,7 @@
       <c r="J146" t="s">
         <v>840</v>
       </c>
-      <c r="K146" t="n">
+      <c r="K146" s="1" t="n">
         <v>43921</v>
       </c>
       <c r="L146"/>
@@ -12644,7 +12650,7 @@
       <c r="J147" t="s">
         <v>22</v>
       </c>
-      <c r="K147" t="n">
+      <c r="K147" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L147" t="s">
@@ -12706,7 +12712,7 @@
       <c r="J148" t="s">
         <v>852</v>
       </c>
-      <c r="K148" t="n">
+      <c r="K148" s="1" t="n">
         <v>43887</v>
       </c>
       <c r="L148"/>
@@ -12766,7 +12772,7 @@
       <c r="J149" t="s">
         <v>862</v>
       </c>
-      <c r="K149" t="n">
+      <c r="K149" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="L149"/>
@@ -12826,7 +12832,7 @@
       <c r="J150" t="s">
         <v>869</v>
       </c>
-      <c r="K150" t="n">
+      <c r="K150" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="L150"/>
@@ -12890,7 +12896,7 @@
       <c r="J151" t="s">
         <v>22</v>
       </c>
-      <c r="K151" t="n">
+      <c r="K151" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L151" t="s">
@@ -12954,7 +12960,7 @@
       <c r="J152" t="s">
         <v>874</v>
       </c>
-      <c r="K152" t="n">
+      <c r="K152" s="1" t="n">
         <v>43888</v>
       </c>
       <c r="L152" t="s">
@@ -13010,7 +13016,7 @@
       <c r="J153" t="s">
         <v>885</v>
       </c>
-      <c r="K153" t="n">
+      <c r="K153" s="1" t="n">
         <v>43895</v>
       </c>
       <c r="L153" t="s">
@@ -13072,7 +13078,7 @@
       <c r="J154" t="s">
         <v>894</v>
       </c>
-      <c r="K154" t="n">
+      <c r="K154" s="1" t="n">
         <v>43895</v>
       </c>
       <c r="L154"/>
@@ -13130,7 +13136,7 @@
       <c r="J155" t="s">
         <v>900</v>
       </c>
-      <c r="K155" t="n">
+      <c r="K155" s="1" t="n">
         <v>43896</v>
       </c>
       <c r="L155" t="s">
@@ -13190,7 +13196,7 @@
       <c r="J156" t="s">
         <v>910</v>
       </c>
-      <c r="K156" t="n">
+      <c r="K156" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="L156" t="s">
@@ -13250,7 +13256,7 @@
       <c r="J157" t="s">
         <v>885</v>
       </c>
-      <c r="K157" t="n">
+      <c r="K157" s="1" t="n">
         <v>43963</v>
       </c>
       <c r="L157"/>
@@ -13308,7 +13314,7 @@
       <c r="J158" t="s">
         <v>924</v>
       </c>
-      <c r="K158" t="n">
+      <c r="K158" s="1" t="n">
         <v>43971</v>
       </c>
       <c r="L158"/>
@@ -13364,7 +13370,7 @@
       <c r="J159" t="s">
         <v>934</v>
       </c>
-      <c r="K159" t="n">
+      <c r="K159" s="1" t="n">
         <v>44018</v>
       </c>
       <c r="L159" t="s">
@@ -13424,7 +13430,7 @@
       <c r="J160" t="s">
         <v>946</v>
       </c>
-      <c r="K160" t="n">
+      <c r="K160" s="1" t="n">
         <v>44021</v>
       </c>
       <c r="L160"/>
@@ -13484,7 +13490,7 @@
       <c r="J161" t="s">
         <v>946</v>
       </c>
-      <c r="K161" t="n">
+      <c r="K161" s="1" t="n">
         <v>44021</v>
       </c>
       <c r="L161"/>
@@ -13544,7 +13550,7 @@
       <c r="J162" t="s">
         <v>955</v>
       </c>
-      <c r="K162" t="n">
+      <c r="K162" s="1" t="n">
         <v>44021</v>
       </c>
       <c r="L162"/>
@@ -13604,7 +13610,7 @@
       <c r="J163" t="s">
         <v>962</v>
       </c>
-      <c r="K163" t="n">
+      <c r="K163" s="1" t="n">
         <v>44026</v>
       </c>
       <c r="L163"/>
@@ -13662,7 +13668,7 @@
       <c r="J164" t="s">
         <v>934</v>
       </c>
-      <c r="K164" t="n">
+      <c r="K164" s="1" t="n">
         <v>44028</v>
       </c>
       <c r="L164"/>
@@ -13720,7 +13726,7 @@
       <c r="J165" t="s">
         <v>934</v>
       </c>
-      <c r="K165" t="n">
+      <c r="K165" s="1" t="n">
         <v>44028</v>
       </c>
       <c r="L165"/>
@@ -13778,7 +13784,7 @@
       <c r="J166" t="s">
         <v>934</v>
       </c>
-      <c r="K166" t="n">
+      <c r="K166" s="1" t="n">
         <v>44028</v>
       </c>
       <c r="L166"/>
@@ -13838,7 +13844,7 @@
       <c r="J167" t="s">
         <v>980</v>
       </c>
-      <c r="K167" t="n">
+      <c r="K167" s="1" t="n">
         <v>44034</v>
       </c>
       <c r="L167"/>
@@ -13898,7 +13904,7 @@
       <c r="J168" t="s">
         <v>980</v>
       </c>
-      <c r="K168" t="n">
+      <c r="K168" s="1" t="n">
         <v>44034</v>
       </c>
       <c r="L168"/>
@@ -13956,7 +13962,7 @@
       <c r="J169" t="s">
         <v>980</v>
       </c>
-      <c r="K169" t="n">
+      <c r="K169" s="1" t="n">
         <v>44067</v>
       </c>
       <c r="L169"/>
@@ -14012,7 +14018,7 @@
       <c r="J170" t="s">
         <v>996</v>
       </c>
-      <c r="K170" t="n">
+      <c r="K170" s="1" t="n">
         <v>44104</v>
       </c>
       <c r="L170"/>
@@ -14062,7 +14068,7 @@
       <c r="J171" t="s">
         <v>999</v>
       </c>
-      <c r="K171" t="n">
+      <c r="K171" s="1" t="n">
         <v>44104</v>
       </c>
       <c r="L171"/>
@@ -14118,7 +14124,7 @@
       <c r="J172" t="s">
         <v>22</v>
       </c>
-      <c r="K172" t="n">
+      <c r="K172" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L172" t="s">
@@ -14184,7 +14190,7 @@
       <c r="J173" t="s">
         <v>369</v>
       </c>
-      <c r="K173" t="n">
+      <c r="K173" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="L173"/>
@@ -14246,7 +14252,7 @@
       <c r="J174" t="s">
         <v>1011</v>
       </c>
-      <c r="K174" t="n">
+      <c r="K174" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="L174"/>
@@ -14306,7 +14312,7 @@
       <c r="J175" t="s">
         <v>76</v>
       </c>
-      <c r="K175" t="n">
+      <c r="K175" s="1" t="n">
         <v>43900</v>
       </c>
       <c r="L175"/>
@@ -14364,7 +14370,7 @@
       <c r="J176" t="s">
         <v>663</v>
       </c>
-      <c r="K176" t="n">
+      <c r="K176" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="L176"/>
@@ -14422,7 +14428,7 @@
       <c r="J177" t="s">
         <v>1011</v>
       </c>
-      <c r="K177" t="n">
+      <c r="K177" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="L177"/>
@@ -14486,7 +14492,7 @@
       <c r="J178" t="s">
         <v>22</v>
       </c>
-      <c r="K178" t="n">
+      <c r="K178" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L178" t="s">
@@ -14554,7 +14560,7 @@
       <c r="J179" t="s">
         <v>22</v>
       </c>
-      <c r="K179" t="n">
+      <c r="K179" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L179" t="s">
@@ -14618,7 +14624,7 @@
       <c r="J180" t="s">
         <v>1036</v>
       </c>
-      <c r="K180" t="n">
+      <c r="K180" s="1" t="n">
         <v>43888</v>
       </c>
       <c r="L180"/>
@@ -14678,7 +14684,7 @@
       <c r="J181" t="s">
         <v>1044</v>
       </c>
-      <c r="K181" t="n">
+      <c r="K181" s="1" t="n">
         <v>43888</v>
       </c>
       <c r="L181"/>
@@ -14742,7 +14748,7 @@
       <c r="J182" t="s">
         <v>22</v>
       </c>
-      <c r="K182" t="n">
+      <c r="K182" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L182" t="s">
@@ -14806,7 +14812,7 @@
       <c r="J183" t="s">
         <v>419</v>
       </c>
-      <c r="K183" t="n">
+      <c r="K183" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L183"/>
@@ -14866,7 +14872,7 @@
       <c r="J184" t="s">
         <v>1055</v>
       </c>
-      <c r="K184" t="n">
+      <c r="K184" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L184"/>
@@ -14924,7 +14930,7 @@
       <c r="J185" t="s">
         <v>1061</v>
       </c>
-      <c r="K185" t="n">
+      <c r="K185" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="L185"/>
@@ -14984,7 +14990,7 @@
       <c r="J186" t="s">
         <v>419</v>
       </c>
-      <c r="K186" t="n">
+      <c r="K186" s="1" t="n">
         <v>43949</v>
       </c>
       <c r="L186"/>
@@ -15044,7 +15050,7 @@
       <c r="J187" t="s">
         <v>278</v>
       </c>
-      <c r="K187" t="n">
+      <c r="K187" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="L187"/>
@@ -15104,7 +15110,7 @@
       <c r="J188" t="s">
         <v>574</v>
       </c>
-      <c r="K188" t="n">
+      <c r="K188" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="L188"/>
@@ -15164,7 +15170,7 @@
       <c r="J189" t="s">
         <v>564</v>
       </c>
-      <c r="K189" t="n">
+      <c r="K189" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="L189"/>
@@ -15222,7 +15228,7 @@
       <c r="J190" t="s">
         <v>192</v>
       </c>
-      <c r="K190" t="n">
+      <c r="K190" s="1" t="n">
         <v>44075</v>
       </c>
       <c r="L190"/>
@@ -15280,7 +15286,7 @@
       <c r="J191" t="s">
         <v>1080</v>
       </c>
-      <c r="K191" t="n">
+      <c r="K191" s="1" t="n">
         <v>44075</v>
       </c>
       <c r="L191"/>
@@ -15344,7 +15350,7 @@
       <c r="J192" t="s">
         <v>22</v>
       </c>
-      <c r="K192" t="n">
+      <c r="K192" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L192" t="s">
@@ -15406,7 +15412,7 @@
       <c r="J193" t="s">
         <v>1085</v>
       </c>
-      <c r="K193" t="n">
+      <c r="K193" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L193"/>
@@ -15462,7 +15468,7 @@
       <c r="J194" t="s">
         <v>1085</v>
       </c>
-      <c r="K194" t="n">
+      <c r="K194" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L194"/>
@@ -15518,7 +15524,7 @@
       <c r="J195" t="s">
         <v>1085</v>
       </c>
-      <c r="K195" t="n">
+      <c r="K195" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L195"/>
@@ -15574,7 +15580,7 @@
       <c r="J196" t="s">
         <v>1094</v>
       </c>
-      <c r="K196" t="n">
+      <c r="K196" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L196"/>
@@ -15630,7 +15636,7 @@
       <c r="J197" t="s">
         <v>1094</v>
       </c>
-      <c r="K197" t="n">
+      <c r="K197" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L197"/>
@@ -15686,7 +15692,7 @@
       <c r="J198" t="s">
         <v>1094</v>
       </c>
-      <c r="K198" t="n">
+      <c r="K198" s="1" t="n">
         <v>43886</v>
       </c>
       <c r="L198"/>
@@ -15744,7 +15750,7 @@
       <c r="J199" t="s">
         <v>419</v>
       </c>
-      <c r="K199" t="n">
+      <c r="K199" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L199"/>
@@ -15804,7 +15810,7 @@
       <c r="J200" t="s">
         <v>1055</v>
       </c>
-      <c r="K200" t="n">
+      <c r="K200" s="1" t="n">
         <v>43893</v>
       </c>
       <c r="L200"/>
@@ -15866,7 +15872,7 @@
       <c r="J201" t="s">
         <v>419</v>
       </c>
-      <c r="K201" t="n">
+      <c r="K201" s="1" t="n">
         <v>43949</v>
       </c>
       <c r="L201"/>
@@ -15930,7 +15936,7 @@
       <c r="J202" t="s">
         <v>22</v>
       </c>
-      <c r="K202" t="n">
+      <c r="K202" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L202" t="s">
@@ -15992,7 +15998,7 @@
       <c r="J203" t="s">
         <v>489</v>
       </c>
-      <c r="K203" t="n">
+      <c r="K203" s="1" t="n">
         <v>43895</v>
       </c>
       <c r="L203"/>
@@ -16050,7 +16056,7 @@
       <c r="J204" t="s">
         <v>1080</v>
       </c>
-      <c r="K204" t="n">
+      <c r="K204" s="1" t="n">
         <v>43895</v>
       </c>
       <c r="L204"/>
@@ -16108,7 +16114,7 @@
       <c r="J205" t="s">
         <v>608</v>
       </c>
-      <c r="K205" t="n">
+      <c r="K205" s="1" t="n">
         <v>43895</v>
       </c>
       <c r="L205"/>
@@ -16166,7 +16172,7 @@
       <c r="J206" t="s">
         <v>130</v>
       </c>
-      <c r="K206" t="n">
+      <c r="K206" s="1" t="n">
         <v>43895</v>
       </c>
       <c r="L206"/>
@@ -16226,7 +16232,7 @@
       <c r="J207" t="s">
         <v>369</v>
       </c>
-      <c r="K207" t="n">
+      <c r="K207" s="1" t="n">
         <v>43922</v>
       </c>
       <c r="L207"/>
@@ -16290,7 +16296,7 @@
       <c r="J208" t="s">
         <v>22</v>
       </c>
-      <c r="K208" t="n">
+      <c r="K208" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L208" t="s">
@@ -16352,7 +16358,7 @@
       <c r="J209" t="s">
         <v>1110</v>
       </c>
-      <c r="K209" t="n">
+      <c r="K209" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="L209"/>
@@ -16410,7 +16416,7 @@
       <c r="J210" t="s">
         <v>1119</v>
       </c>
-      <c r="K210" t="n">
+      <c r="K210" s="1" t="n">
         <v>43938</v>
       </c>
       <c r="L210"/>
@@ -16468,7 +16474,7 @@
       <c r="J211" t="s">
         <v>119</v>
       </c>
-      <c r="K211" t="n">
+      <c r="K211" s="1" t="n">
         <v>43942</v>
       </c>
       <c r="L211"/>
@@ -16528,7 +16534,7 @@
       <c r="J212" t="s">
         <v>1128</v>
       </c>
-      <c r="K212" t="n">
+      <c r="K212" s="1" t="n">
         <v>44042</v>
       </c>
       <c r="L212"/>
@@ -16588,7 +16594,7 @@
       <c r="J213" t="s">
         <v>1135</v>
       </c>
-      <c r="K213" t="n">
+      <c r="K213" s="1" t="n">
         <v>44042</v>
       </c>
       <c r="L213"/>
@@ -16648,7 +16654,7 @@
       <c r="J214" t="s">
         <v>1137</v>
       </c>
-      <c r="K214" t="n">
+      <c r="K214" s="1" t="n">
         <v>44042</v>
       </c>
       <c r="L214"/>
@@ -16708,7 +16714,7 @@
       <c r="J215" t="s">
         <v>1139</v>
       </c>
-      <c r="K215" t="n">
+      <c r="K215" s="1" t="n">
         <v>44042</v>
       </c>
       <c r="L215"/>
@@ -16766,7 +16772,7 @@
       <c r="J216" t="s">
         <v>1143</v>
       </c>
-      <c r="K216" t="n">
+      <c r="K216" s="1" t="n">
         <v>44047</v>
       </c>
       <c r="L216"/>
@@ -16824,7 +16830,7 @@
       <c r="J217" t="s">
         <v>1152</v>
       </c>
-      <c r="K217" t="n">
+      <c r="K217" s="1" t="n">
         <v>44061</v>
       </c>
       <c r="L217"/>
@@ -16882,7 +16888,7 @@
       <c r="J218" t="s">
         <v>1139</v>
       </c>
-      <c r="K218" t="n">
+      <c r="K218" s="1" t="n">
         <v>44061</v>
       </c>
       <c r="L218"/>

</xml_diff>